<commit_message>
images on administrator panel
</commit_message>
<xml_diff>
--- a/allusers.xlsx
+++ b/allusers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -103,33 +103,6 @@
     <t>2019-03-17</t>
   </si>
   <si>
-    <t>Мулькин</t>
-  </si>
-  <si>
-    <t>Певел</t>
-  </si>
-  <si>
-    <t>Сергеевич</t>
-  </si>
-  <si>
-    <t>ЮрФУ</t>
-  </si>
-  <si>
-    <t>patro1@yandex.ru</t>
-  </si>
-  <si>
-    <t>223-322-223</t>
-  </si>
-  <si>
-    <t>11.11.2011</t>
-  </si>
-  <si>
-    <t>mul</t>
-  </si>
-  <si>
-    <t>2019-03-24</t>
-  </si>
-  <si>
     <t>Мрак</t>
   </si>
   <si>
@@ -157,28 +130,7 @@
     <t>2019-04-28</t>
   </si>
   <si>
-    <t>Холостов</t>
-  </si>
-  <si>
-    <t>Петрович</t>
-  </si>
-  <si>
-    <t>ФП</t>
-  </si>
-  <si>
-    <t>4585</t>
-  </si>
-  <si>
-    <t>25.11.1962</t>
-  </si>
-  <si>
-    <t>uup</t>
-  </si>
-  <si>
-    <t>2019-05-10</t>
-  </si>
-  <si>
-    <t>2019-07-26 00:00:00</t>
+    <t>2019-08-03 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -510,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -623,7 +575,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -657,78 +609,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>